<commit_message>
revised the entire paper
</commit_message>
<xml_diff>
--- a/src/bibtex/bib/sorted_references_linked.xlsx
+++ b/src/bibtex/bib/sorted_references_linked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://malayancollegesmindanaoo365-my.sharepoint.com/personal/vatomas_mcm_edu_ph/Documents/School/Capstone/MoR/src/bibtex/bib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{437714D0-950C-4073-ACE5-4CF54E2DC04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEF8018B-2721-4A7A-BA71-83890E55A145}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{437714D0-950C-4073-ACE5-4CF54E2DC04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C600D3-09FB-4389-B06A-54498743EC32}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2FCC965B-A4A8-49B7-B936-B627D6D09D7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{2FCC965B-A4A8-49B7-B936-B627D6D09D7F}"/>
   </bookViews>
   <sheets>
     <sheet name="sorted_references_linked" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t>Antonnete Number</t>
   </si>
@@ -635,6 +635,15 @@
   </si>
   <si>
     <t>Science Driect ID</t>
+  </si>
+  <si>
+    <t>Av2</t>
+  </si>
+  <si>
+    <t>Tv2</t>
+  </si>
+  <si>
+    <t>Av1</t>
   </si>
 </sst>
 </file>
@@ -676,7 +685,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -698,9 +714,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -738,7 +754,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -844,7 +860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -986,7 +1002,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -994,137 +1010,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F828D77-A6CD-41F1-9241-6B5522377CD0}">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" customWidth="1"/>
-    <col min="12" max="12" width="0.21875" customWidth="1"/>
-    <col min="13" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="0.21875" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>80</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>82</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
+      <c r="K2" t="b">
         <v>1</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>120</v>
       </c>
-      <c r="P2" t="str">
-        <f>"\cite{" &amp;C2 &amp; "} &amp; " &amp; IF(E2,"\checkmark","") &amp; " &amp; "&amp; IF(F2,"\checkmark","") &amp; " &amp; "&amp; IF(G2,"\checkmark","") &amp; " &amp; "&amp; IF(H2,"\checkmark","") &amp; " &amp; "&amp; IF(I2,"\checkmark","") &amp; " &amp; "&amp; IF(J2,"\checkmark","") &amp; " &amp; "&amp; IF(K2,"\checkmark","") &amp; " &amp; "&amp; IF(L2,"\checkmark","") &amp; " &amp; "&amp; IF(M2,"\checkmark","") &amp; " &amp; "&amp; IF(N2,"\checkmark","") &amp; " \\"</f>
+      <c r="R2" t="str">
+        <f>"\cite{" &amp;E2 &amp; "} &amp; " &amp; IF(G2,"\checkmark","") &amp; " &amp; "&amp; IF(H2,"\checkmark","") &amp; " &amp; "&amp; IF(I2,"\checkmark","") &amp; " &amp; "&amp; IF(J2,"\checkmark","") &amp; " &amp; "&amp; IF(K2,"\checkmark","") &amp; " &amp; "&amp; IF(L2,"\checkmark","") &amp; " &amp; "&amp; IF(M2,"\checkmark","") &amp; " &amp; "&amp; IF(N2,"\checkmark","") &amp; " &amp; "&amp; IF(O2,"\checkmark","") &amp; " &amp; "&amp; IF(P2,"\checkmark","") &amp; " \\"</f>
         <v>\cite{kang_robotic-based_2021} &amp; \checkmark &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE2" t="str">
-        <f>"https://doi.org/" &amp; B2</f>
+      <c r="AG2" t="str">
+        <f>"https://doi.org/" &amp; D2</f>
         <v>https://doi.org/10.1016/j.ndteint.2021.102500</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
@@ -1137,75 +1164,81 @@
       <c r="N3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>121</v>
       </c>
-      <c r="P3" t="str">
-        <f>"\cite{" &amp;C3 &amp; "} &amp; " &amp; IF(E3,"\checkmark","") &amp; " &amp; "&amp; IF(F3,"\checkmark","") &amp; " &amp; "&amp; IF(G3,"\checkmark","") &amp; " &amp; "&amp; IF(H3,"\checkmark","") &amp; " &amp; "&amp; IF(I3,"\checkmark","") &amp; " &amp; "&amp; IF(J3,"\checkmark","") &amp; " &amp; "&amp; IF(K3,"\checkmark","") &amp; " &amp; "&amp; IF(L3,"\checkmark","") &amp; " &amp; "&amp; IF(M3,"\checkmark","") &amp; " &amp; "&amp; IF(N3,"\checkmark","") &amp; " \\"</f>
+      <c r="R3" t="str">
+        <f>"\cite{" &amp;E3 &amp; "} &amp; " &amp; IF(G3,"\checkmark","") &amp; " &amp; "&amp; IF(H3,"\checkmark","") &amp; " &amp; "&amp; IF(I3,"\checkmark","") &amp; " &amp; "&amp; IF(J3,"\checkmark","") &amp; " &amp; "&amp; IF(K3,"\checkmark","") &amp; " &amp; "&amp; IF(L3,"\checkmark","") &amp; " &amp; "&amp; IF(M3,"\checkmark","") &amp; " &amp; "&amp; IF(N3,"\checkmark","") &amp; " &amp; "&amp; IF(O3,"\checkmark","") &amp; " &amp; "&amp; IF(P3,"\checkmark","") &amp; " \\"</f>
         <v>\cite{yang_broadband_2023} &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE3" t="str">
-        <f>"https://doi.org/" &amp; B3</f>
+      <c r="AG3" t="str">
+        <f>"https://doi.org/" &amp; D3</f>
         <v>https://doi.org/10.1016/j.sna.2023.114819</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
+      <c r="G4" t="b">
         <v>1</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>157</v>
       </c>
-      <c r="P4" t="str">
-        <f>"\cite{" &amp;C4 &amp; "} &amp; " &amp; IF(E4,"\checkmark","") &amp; " &amp; "&amp; IF(F4,"\checkmark","") &amp; " &amp; "&amp; IF(G4,"\checkmark","") &amp; " &amp; "&amp; IF(H4,"\checkmark","") &amp; " &amp; "&amp; IF(I4,"\checkmark","") &amp; " &amp; "&amp; IF(J4,"\checkmark","") &amp; " &amp; "&amp; IF(K4,"\checkmark","") &amp; " &amp; "&amp; IF(L4,"\checkmark","") &amp; " &amp; "&amp; IF(M4,"\checkmark","") &amp; " &amp; "&amp; IF(N4,"\checkmark","") &amp; " \\"</f>
+      <c r="R4" t="str">
+        <f>"\cite{" &amp;E4 &amp; "} &amp; " &amp; IF(G4,"\checkmark","") &amp; " &amp; "&amp; IF(H4,"\checkmark","") &amp; " &amp; "&amp; IF(I4,"\checkmark","") &amp; " &amp; "&amp; IF(J4,"\checkmark","") &amp; " &amp; "&amp; IF(K4,"\checkmark","") &amp; " &amp; "&amp; IF(L4,"\checkmark","") &amp; " &amp; "&amp; IF(M4,"\checkmark","") &amp; " &amp; "&amp; IF(N4,"\checkmark","") &amp; " &amp; "&amp; IF(O4,"\checkmark","") &amp; " &amp; "&amp; IF(P4,"\checkmark","") &amp; " \\"</f>
         <v>\cite{prasad_real-time_2024} &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp;  \\</v>
       </c>
-      <c r="AE4" t="str">
-        <f>"https://doi.org/" &amp; B4</f>
+      <c r="AG4" t="str">
+        <f>"https://doi.org/" &amp; D4</f>
         <v>https://doi.org/10.1016/j.measurement.2024.114222</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="b">
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="L5" t="b">
@@ -1214,197 +1247,227 @@
       <c r="N5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
         <v>158</v>
       </c>
-      <c r="P5" t="str">
-        <f>"\cite{" &amp;C5 &amp; "} &amp; " &amp; IF(E5,"\checkmark","") &amp; " &amp; "&amp; IF(F5,"\checkmark","") &amp; " &amp; "&amp; IF(G5,"\checkmark","") &amp; " &amp; "&amp; IF(H5,"\checkmark","") &amp; " &amp; "&amp; IF(I5,"\checkmark","") &amp; " &amp; "&amp; IF(J5,"\checkmark","") &amp; " &amp; "&amp; IF(K5,"\checkmark","") &amp; " &amp; "&amp; IF(L5,"\checkmark","") &amp; " &amp; "&amp; IF(M5,"\checkmark","") &amp; " &amp; "&amp; IF(N5,"\checkmark","") &amp; " \\"</f>
+      <c r="R5" t="str">
+        <f>"\cite{" &amp;E5 &amp; "} &amp; " &amp; IF(G5,"\checkmark","") &amp; " &amp; "&amp; IF(H5,"\checkmark","") &amp; " &amp; "&amp; IF(I5,"\checkmark","") &amp; " &amp; "&amp; IF(J5,"\checkmark","") &amp; " &amp; "&amp; IF(K5,"\checkmark","") &amp; " &amp; "&amp; IF(L5,"\checkmark","") &amp; " &amp; "&amp; IF(M5,"\checkmark","") &amp; " &amp; "&amp; IF(N5,"\checkmark","") &amp; " &amp; "&amp; IF(O5,"\checkmark","") &amp; " &amp; "&amp; IF(P5,"\checkmark","") &amp; " \\"</f>
         <v>\cite{cawley_guided_2024} &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE5" t="str">
-        <f>"https://doi.org/" &amp; B5</f>
+      <c r="AG5" t="str">
+        <f>"https://doi.org/" &amp; D5</f>
         <v>https://doi.org/10.1016/j.ndteint.2023.103026</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
       <c r="G6" t="b">
         <v>1</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
         <v>159</v>
       </c>
-      <c r="P6" t="str">
-        <f>"\cite{" &amp;C6 &amp; "} &amp; " &amp; IF(E6,"\checkmark","") &amp; " &amp; "&amp; IF(F6,"\checkmark","") &amp; " &amp; "&amp; IF(G6,"\checkmark","") &amp; " &amp; "&amp; IF(H6,"\checkmark","") &amp; " &amp; "&amp; IF(I6,"\checkmark","") &amp; " &amp; "&amp; IF(J6,"\checkmark","") &amp; " &amp; "&amp; IF(K6,"\checkmark","") &amp; " &amp; "&amp; IF(L6,"\checkmark","") &amp; " &amp; "&amp; IF(M6,"\checkmark","") &amp; " &amp; "&amp; IF(N6,"\checkmark","") &amp; " \\"</f>
+      <c r="R6" t="str">
+        <f>"\cite{" &amp;E6 &amp; "} &amp; " &amp; IF(G6,"\checkmark","") &amp; " &amp; "&amp; IF(H6,"\checkmark","") &amp; " &amp; "&amp; IF(I6,"\checkmark","") &amp; " &amp; "&amp; IF(J6,"\checkmark","") &amp; " &amp; "&amp; IF(K6,"\checkmark","") &amp; " &amp; "&amp; IF(L6,"\checkmark","") &amp; " &amp; "&amp; IF(M6,"\checkmark","") &amp; " &amp; "&amp; IF(N6,"\checkmark","") &amp; " &amp; "&amp; IF(O6,"\checkmark","") &amp; " &amp; "&amp; IF(P6,"\checkmark","") &amp; " \\"</f>
         <v>\cite{moradi_intelligent_2023} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE6" t="str">
-        <f>"https://doi.org/" &amp; B6</f>
+      <c r="AG6" t="str">
+        <f>"https://doi.org/" &amp; D6</f>
         <v>https://doi.org/10.1016/j.engappai.2022.105502</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="b">
+      <c r="J7" t="b">
         <v>1</v>
       </c>
       <c r="N7" t="b">
         <v>1</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
         <v>160</v>
       </c>
-      <c r="P7" t="str">
-        <f>"\cite{" &amp;C7 &amp; "} &amp; " &amp; IF(E7,"\checkmark","") &amp; " &amp; "&amp; IF(F7,"\checkmark","") &amp; " &amp; "&amp; IF(G7,"\checkmark","") &amp; " &amp; "&amp; IF(H7,"\checkmark","") &amp; " &amp; "&amp; IF(I7,"\checkmark","") &amp; " &amp; "&amp; IF(J7,"\checkmark","") &amp; " &amp; "&amp; IF(K7,"\checkmark","") &amp; " &amp; "&amp; IF(L7,"\checkmark","") &amp; " &amp; "&amp; IF(M7,"\checkmark","") &amp; " &amp; "&amp; IF(N7,"\checkmark","") &amp; " \\"</f>
+      <c r="R7" t="str">
+        <f>"\cite{" &amp;E7 &amp; "} &amp; " &amp; IF(G7,"\checkmark","") &amp; " &amp; "&amp; IF(H7,"\checkmark","") &amp; " &amp; "&amp; IF(I7,"\checkmark","") &amp; " &amp; "&amp; IF(J7,"\checkmark","") &amp; " &amp; "&amp; IF(K7,"\checkmark","") &amp; " &amp; "&amp; IF(L7,"\checkmark","") &amp; " &amp; "&amp; IF(M7,"\checkmark","") &amp; " &amp; "&amp; IF(N7,"\checkmark","") &amp; " &amp; "&amp; IF(O7,"\checkmark","") &amp; " &amp; "&amp; IF(P7,"\checkmark","") &amp; " \\"</f>
         <v>\cite{ziaja_shm_2021} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE7" t="str">
-        <f>"https://doi.org/" &amp; B7</f>
+      <c r="AG7" t="str">
+        <f>"https://doi.org/" &amp; D7</f>
         <v>https://doi.org/10.1016/j.istruc.2021.06.086</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>7</v>
       </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
       <c r="J8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
       <c r="L8" t="b">
         <v>1</v>
       </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
       <c r="N8" t="b">
         <v>1</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
         <v>161</v>
       </c>
-      <c r="P8" t="str">
-        <f>"\cite{" &amp;C8 &amp; "} &amp; " &amp; IF(E8,"\checkmark","") &amp; " &amp; "&amp; IF(F8,"\checkmark","") &amp; " &amp; "&amp; IF(G8,"\checkmark","") &amp; " &amp; "&amp; IF(H8,"\checkmark","") &amp; " &amp; "&amp; IF(I8,"\checkmark","") &amp; " &amp; "&amp; IF(J8,"\checkmark","") &amp; " &amp; "&amp; IF(K8,"\checkmark","") &amp; " &amp; "&amp; IF(L8,"\checkmark","") &amp; " &amp; "&amp; IF(M8,"\checkmark","") &amp; " &amp; "&amp; IF(N8,"\checkmark","") &amp; " \\"</f>
+      <c r="R8" t="str">
+        <f>"\cite{" &amp;E8 &amp; "} &amp; " &amp; IF(G8,"\checkmark","") &amp; " &amp; "&amp; IF(H8,"\checkmark","") &amp; " &amp; "&amp; IF(I8,"\checkmark","") &amp; " &amp; "&amp; IF(J8,"\checkmark","") &amp; " &amp; "&amp; IF(K8,"\checkmark","") &amp; " &amp; "&amp; IF(L8,"\checkmark","") &amp; " &amp; "&amp; IF(M8,"\checkmark","") &amp; " &amp; "&amp; IF(N8,"\checkmark","") &amp; " &amp; "&amp; IF(O8,"\checkmark","") &amp; " &amp; "&amp; IF(P8,"\checkmark","") &amp; " \\"</f>
         <v>\cite{katunin_modeling_2021} &amp;  &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE8" t="str">
-        <f>"https://doi.org/" &amp; B8</f>
+      <c r="AG8" t="str">
+        <f>"https://doi.org/" &amp; D8</f>
         <v>https://doi.org/10.1016/j.compstruct.2021.113889</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>8</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" t="b">
+      <c r="K9" t="b">
         <v>1</v>
       </c>
       <c r="N9" t="b">
         <v>1</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
         <v>162</v>
       </c>
-      <c r="P9" t="str">
-        <f>"\cite{" &amp;C9 &amp; "} &amp; " &amp; IF(E9,"\checkmark","") &amp; " &amp; "&amp; IF(F9,"\checkmark","") &amp; " &amp; "&amp; IF(G9,"\checkmark","") &amp; " &amp; "&amp; IF(H9,"\checkmark","") &amp; " &amp; "&amp; IF(I9,"\checkmark","") &amp; " &amp; "&amp; IF(J9,"\checkmark","") &amp; " &amp; "&amp; IF(K9,"\checkmark","") &amp; " &amp; "&amp; IF(L9,"\checkmark","") &amp; " &amp; "&amp; IF(M9,"\checkmark","") &amp; " &amp; "&amp; IF(N9,"\checkmark","") &amp; " \\"</f>
+      <c r="R9" t="str">
+        <f>"\cite{" &amp;E9 &amp; "} &amp; " &amp; IF(G9,"\checkmark","") &amp; " &amp; "&amp; IF(H9,"\checkmark","") &amp; " &amp; "&amp; IF(I9,"\checkmark","") &amp; " &amp; "&amp; IF(J9,"\checkmark","") &amp; " &amp; "&amp; IF(K9,"\checkmark","") &amp; " &amp; "&amp; IF(L9,"\checkmark","") &amp; " &amp; "&amp; IF(M9,"\checkmark","") &amp; " &amp; "&amp; IF(N9,"\checkmark","") &amp; " &amp; "&amp; IF(O9,"\checkmark","") &amp; " &amp; "&amp; IF(P9,"\checkmark","") &amp; " \\"</f>
         <v>\cite{carcione_demodulation_2020} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE9" t="str">
-        <f>"https://doi.org/" &amp; B9</f>
+      <c r="AG9" t="str">
+        <f>"https://doi.org/" &amp; D9</f>
         <v>https://doi.org/10.1016/j.jsv.2019.115014</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>9</v>
       </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
       <c r="H10" t="b">
         <v>1</v>
       </c>
@@ -1417,112 +1480,127 @@
       <c r="N10" t="b">
         <v>1</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
         <v>163</v>
       </c>
-      <c r="P10" t="str">
-        <f>"\cite{" &amp;C10 &amp; "} &amp; " &amp; IF(E10,"\checkmark","") &amp; " &amp; "&amp; IF(F10,"\checkmark","") &amp; " &amp; "&amp; IF(G10,"\checkmark","") &amp; " &amp; "&amp; IF(H10,"\checkmark","") &amp; " &amp; "&amp; IF(I10,"\checkmark","") &amp; " &amp; "&amp; IF(J10,"\checkmark","") &amp; " &amp; "&amp; IF(K10,"\checkmark","") &amp; " &amp; "&amp; IF(L10,"\checkmark","") &amp; " &amp; "&amp; IF(M10,"\checkmark","") &amp; " &amp; "&amp; IF(N10,"\checkmark","") &amp; " \\"</f>
+      <c r="R10" t="str">
+        <f>"\cite{" &amp;E10 &amp; "} &amp; " &amp; IF(G10,"\checkmark","") &amp; " &amp; "&amp; IF(H10,"\checkmark","") &amp; " &amp; "&amp; IF(I10,"\checkmark","") &amp; " &amp; "&amp; IF(J10,"\checkmark","") &amp; " &amp; "&amp; IF(K10,"\checkmark","") &amp; " &amp; "&amp; IF(L10,"\checkmark","") &amp; " &amp; "&amp; IF(M10,"\checkmark","") &amp; " &amp; "&amp; IF(N10,"\checkmark","") &amp; " &amp; "&amp; IF(O10,"\checkmark","") &amp; " &amp; "&amp; IF(P10,"\checkmark","") &amp; " \\"</f>
         <v>\cite{balasubramaniam_multi_2022} &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE10" t="str">
-        <f>"https://doi.org/" &amp; B10</f>
+      <c r="AG10" t="str">
+        <f>"https://doi.org/" &amp; D10</f>
         <v>https://doi.org/10.1016/j.measurement.2022.111057</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>10</v>
       </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
         <v>164</v>
       </c>
-      <c r="P11" t="str">
-        <f>"\cite{" &amp;C11 &amp; "} &amp; " &amp; IF(E11,"\checkmark","") &amp; " &amp; "&amp; IF(F11,"\checkmark","") &amp; " &amp; "&amp; IF(G11,"\checkmark","") &amp; " &amp; "&amp; IF(H11,"\checkmark","") &amp; " &amp; "&amp; IF(I11,"\checkmark","") &amp; " &amp; "&amp; IF(J11,"\checkmark","") &amp; " &amp; "&amp; IF(K11,"\checkmark","") &amp; " &amp; "&amp; IF(L11,"\checkmark","") &amp; " &amp; "&amp; IF(M11,"\checkmark","") &amp; " &amp; "&amp; IF(N11,"\checkmark","") &amp; " \\"</f>
+      <c r="R11" t="str">
+        <f>"\cite{" &amp;E11 &amp; "} &amp; " &amp; IF(G11,"\checkmark","") &amp; " &amp; "&amp; IF(H11,"\checkmark","") &amp; " &amp; "&amp; IF(I11,"\checkmark","") &amp; " &amp; "&amp; IF(J11,"\checkmark","") &amp; " &amp; "&amp; IF(K11,"\checkmark","") &amp; " &amp; "&amp; IF(L11,"\checkmark","") &amp; " &amp; "&amp; IF(M11,"\checkmark","") &amp; " &amp; "&amp; IF(N11,"\checkmark","") &amp; " &amp; "&amp; IF(O11,"\checkmark","") &amp; " &amp; "&amp; IF(P11,"\checkmark","") &amp; " \\"</f>
         <v>\cite{lambinet_measurement_2022} &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark &amp;  &amp;  &amp;  &amp;  &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE11" t="str">
-        <f>"https://doi.org/" &amp; B11</f>
+      <c r="AG11" t="str">
+        <f>"https://doi.org/" &amp; D11</f>
         <v>https://doi.org/10.1016/j.measurement.2021.110675</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>11</v>
       </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
         <v>165</v>
       </c>
-      <c r="P12" t="str">
-        <f>"\cite{" &amp;C12 &amp; "} &amp; " &amp; IF(E12,"\checkmark","") &amp; " &amp; "&amp; IF(F12,"\checkmark","") &amp; " &amp; "&amp; IF(G12,"\checkmark","") &amp; " &amp; "&amp; IF(H12,"\checkmark","") &amp; " &amp; "&amp; IF(I12,"\checkmark","") &amp; " &amp; "&amp; IF(J12,"\checkmark","") &amp; " &amp; "&amp; IF(K12,"\checkmark","") &amp; " &amp; "&amp; IF(L12,"\checkmark","") &amp; " &amp; "&amp; IF(M12,"\checkmark","") &amp; " &amp; "&amp; IF(N12,"\checkmark","") &amp; " \\"</f>
+      <c r="R12" t="str">
+        <f>"\cite{" &amp;E12 &amp; "} &amp; " &amp; IF(G12,"\checkmark","") &amp; " &amp; "&amp; IF(H12,"\checkmark","") &amp; " &amp; "&amp; IF(I12,"\checkmark","") &amp; " &amp; "&amp; IF(J12,"\checkmark","") &amp; " &amp; "&amp; IF(K12,"\checkmark","") &amp; " &amp; "&amp; IF(L12,"\checkmark","") &amp; " &amp; "&amp; IF(M12,"\checkmark","") &amp; " &amp; "&amp; IF(N12,"\checkmark","") &amp; " &amp; "&amp; IF(O12,"\checkmark","") &amp; " &amp; "&amp; IF(P12,"\checkmark","") &amp; " \\"</f>
         <v>\cite{rehman_advancing_2024} &amp; \checkmark &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE12" t="str">
-        <f>"https://doi.org/" &amp; B12</f>
+      <c r="AG12" t="str">
+        <f>"https://doi.org/" &amp; D12</f>
         <v>https://doi.org/10.1016/j.sna.2023.114863</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>49</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
+      <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="b">
@@ -1531,535 +1609,607 @@
       <c r="L13" t="b">
         <v>1</v>
       </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
         <v>166</v>
       </c>
-      <c r="P13" t="str">
-        <f>"\cite{" &amp;C13 &amp; "} &amp; " &amp; IF(E13,"\checkmark","") &amp; " &amp; "&amp; IF(F13,"\checkmark","") &amp; " &amp; "&amp; IF(G13,"\checkmark","") &amp; " &amp; "&amp; IF(H13,"\checkmark","") &amp; " &amp; "&amp; IF(I13,"\checkmark","") &amp; " &amp; "&amp; IF(J13,"\checkmark","") &amp; " &amp; "&amp; IF(K13,"\checkmark","") &amp; " &amp; "&amp; IF(L13,"\checkmark","") &amp; " &amp; "&amp; IF(M13,"\checkmark","") &amp; " &amp; "&amp; IF(N13,"\checkmark","") &amp; " \\"</f>
+      <c r="R13" t="str">
+        <f>"\cite{" &amp;E13 &amp; "} &amp; " &amp; IF(G13,"\checkmark","") &amp; " &amp; "&amp; IF(H13,"\checkmark","") &amp; " &amp; "&amp; IF(I13,"\checkmark","") &amp; " &amp; "&amp; IF(J13,"\checkmark","") &amp; " &amp; "&amp; IF(K13,"\checkmark","") &amp; " &amp; "&amp; IF(L13,"\checkmark","") &amp; " &amp; "&amp; IF(M13,"\checkmark","") &amp; " &amp; "&amp; IF(N13,"\checkmark","") &amp; " &amp; "&amp; IF(O13,"\checkmark","") &amp; " &amp; "&amp; IF(P13,"\checkmark","") &amp; " \\"</f>
         <v>\cite{carani_impact_2022} &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE13" t="str">
-        <f>"https://doi.org/" &amp; B13</f>
+      <c r="AG13" t="str">
+        <f>"https://doi.org/" &amp; D13</f>
         <v>https://doi.org/10.1016/j.sna.2022.113843</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>50</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>13</v>
       </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
+      <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" t="b">
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
         <v>1</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
         <v>167</v>
       </c>
-      <c r="P14" t="str">
-        <f>"\cite{" &amp;C14 &amp; "} &amp; " &amp; IF(E14,"\checkmark","") &amp; " &amp; "&amp; IF(F14,"\checkmark","") &amp; " &amp; "&amp; IF(G14,"\checkmark","") &amp; " &amp; "&amp; IF(H14,"\checkmark","") &amp; " &amp; "&amp; IF(I14,"\checkmark","") &amp; " &amp; "&amp; IF(J14,"\checkmark","") &amp; " &amp; "&amp; IF(K14,"\checkmark","") &amp; " &amp; "&amp; IF(L14,"\checkmark","") &amp; " &amp; "&amp; IF(M14,"\checkmark","") &amp; " &amp; "&amp; IF(N14,"\checkmark","") &amp; " \\"</f>
+      <c r="R14" t="str">
+        <f>"\cite{" &amp;E14 &amp; "} &amp; " &amp; IF(G14,"\checkmark","") &amp; " &amp; "&amp; IF(H14,"\checkmark","") &amp; " &amp; "&amp; IF(I14,"\checkmark","") &amp; " &amp; "&amp; IF(J14,"\checkmark","") &amp; " &amp; "&amp; IF(K14,"\checkmark","") &amp; " &amp; "&amp; IF(L14,"\checkmark","") &amp; " &amp; "&amp; IF(M14,"\checkmark","") &amp; " &amp; "&amp; IF(N14,"\checkmark","") &amp; " &amp; "&amp; IF(O14,"\checkmark","") &amp; " &amp; "&amp; IF(P14,"\checkmark","") &amp; " \\"</f>
         <v>\cite{sanchez-romate_structural_2021} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE14" t="str">
-        <f>"https://doi.org/" &amp; B14</f>
+      <c r="AG14" t="str">
+        <f>"https://doi.org/" &amp; D14</f>
         <v>https://doi.org/10.1016/j.compstruct.2021.114091</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>14</v>
       </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
       <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-      <c r="M15" t="b">
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
         <v>168</v>
       </c>
-      <c r="P15" t="str">
-        <f>"\cite{" &amp;C15 &amp; "} &amp; " &amp; IF(E15,"\checkmark","") &amp; " &amp; "&amp; IF(F15,"\checkmark","") &amp; " &amp; "&amp; IF(G15,"\checkmark","") &amp; " &amp; "&amp; IF(H15,"\checkmark","") &amp; " &amp; "&amp; IF(I15,"\checkmark","") &amp; " &amp; "&amp; IF(J15,"\checkmark","") &amp; " &amp; "&amp; IF(K15,"\checkmark","") &amp; " &amp; "&amp; IF(L15,"\checkmark","") &amp; " &amp; "&amp; IF(M15,"\checkmark","") &amp; " &amp; "&amp; IF(N15,"\checkmark","") &amp; " \\"</f>
+      <c r="R15" t="str">
+        <f>"\cite{" &amp;E15 &amp; "} &amp; " &amp; IF(G15,"\checkmark","") &amp; " &amp; "&amp; IF(H15,"\checkmark","") &amp; " &amp; "&amp; IF(I15,"\checkmark","") &amp; " &amp; "&amp; IF(J15,"\checkmark","") &amp; " &amp; "&amp; IF(K15,"\checkmark","") &amp; " &amp; "&amp; IF(L15,"\checkmark","") &amp; " &amp; "&amp; IF(M15,"\checkmark","") &amp; " &amp; "&amp; IF(N15,"\checkmark","") &amp; " &amp; "&amp; IF(O15,"\checkmark","") &amp; " &amp; "&amp; IF(P15,"\checkmark","") &amp; " \\"</f>
         <v>\cite{zhang_spatial_2023} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE15" t="str">
-        <f>"https://doi.org/" &amp; B15</f>
+      <c r="AG15" t="str">
+        <f>"https://doi.org/" &amp; D15</f>
         <v>https://doi.org/10.1016/j.jsv.2023.117636</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>52</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>15</v>
       </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
+      <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
-      <c r="L16" t="b">
+      <c r="J16" t="b">
         <v>1</v>
       </c>
       <c r="N16" t="b">
         <v>1</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
         <v>169</v>
       </c>
-      <c r="P16" t="str">
-        <f>"\cite{" &amp;C16 &amp; "} &amp; " &amp; IF(E16,"\checkmark","") &amp; " &amp; "&amp; IF(F16,"\checkmark","") &amp; " &amp; "&amp; IF(G16,"\checkmark","") &amp; " &amp; "&amp; IF(H16,"\checkmark","") &amp; " &amp; "&amp; IF(I16,"\checkmark","") &amp; " &amp; "&amp; IF(J16,"\checkmark","") &amp; " &amp; "&amp; IF(K16,"\checkmark","") &amp; " &amp; "&amp; IF(L16,"\checkmark","") &amp; " &amp; "&amp; IF(M16,"\checkmark","") &amp; " &amp; "&amp; IF(N16,"\checkmark","") &amp; " \\"</f>
+      <c r="R16" t="str">
+        <f>"\cite{" &amp;E16 &amp; "} &amp; " &amp; IF(G16,"\checkmark","") &amp; " &amp; "&amp; IF(H16,"\checkmark","") &amp; " &amp; "&amp; IF(I16,"\checkmark","") &amp; " &amp; "&amp; IF(J16,"\checkmark","") &amp; " &amp; "&amp; IF(K16,"\checkmark","") &amp; " &amp; "&amp; IF(L16,"\checkmark","") &amp; " &amp; "&amp; IF(M16,"\checkmark","") &amp; " &amp; "&amp; IF(N16,"\checkmark","") &amp; " &amp; "&amp; IF(O16,"\checkmark","") &amp; " &amp; "&amp; IF(P16,"\checkmark","") &amp; " \\"</f>
         <v>\cite{parida_comparative_2023} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE16" t="str">
-        <f>"https://doi.org/" &amp; B16</f>
+      <c r="AG16" t="str">
+        <f>"https://doi.org/" &amp; D16</f>
         <v>https://doi.org/10.1016/j.measurement.2023.113592</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>16</v>
       </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
-      <c r="J17" t="b">
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
       </c>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
-      <c r="O17" t="s">
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
         <v>170</v>
       </c>
-      <c r="P17" t="str">
-        <f>"\cite{" &amp;C17 &amp; "} &amp; " &amp; IF(E17,"\checkmark","") &amp; " &amp; "&amp; IF(F17,"\checkmark","") &amp; " &amp; "&amp; IF(G17,"\checkmark","") &amp; " &amp; "&amp; IF(H17,"\checkmark","") &amp; " &amp; "&amp; IF(I17,"\checkmark","") &amp; " &amp; "&amp; IF(J17,"\checkmark","") &amp; " &amp; "&amp; IF(K17,"\checkmark","") &amp; " &amp; "&amp; IF(L17,"\checkmark","") &amp; " &amp; "&amp; IF(M17,"\checkmark","") &amp; " &amp; "&amp; IF(N17,"\checkmark","") &amp; " \\"</f>
+      <c r="R17" t="str">
+        <f>"\cite{" &amp;E17 &amp; "} &amp; " &amp; IF(G17,"\checkmark","") &amp; " &amp; "&amp; IF(H17,"\checkmark","") &amp; " &amp; "&amp; IF(I17,"\checkmark","") &amp; " &amp; "&amp; IF(J17,"\checkmark","") &amp; " &amp; "&amp; IF(K17,"\checkmark","") &amp; " &amp; "&amp; IF(L17,"\checkmark","") &amp; " &amp; "&amp; IF(M17,"\checkmark","") &amp; " &amp; "&amp; IF(N17,"\checkmark","") &amp; " &amp; "&amp; IF(O17,"\checkmark","") &amp; " &amp; "&amp; IF(P17,"\checkmark","") &amp; " \\"</f>
         <v>\cite{rufai_cure_2020} &amp; \checkmark &amp; \checkmark &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE17" t="str">
-        <f>"https://doi.org/" &amp; B17</f>
+      <c r="AG17" t="str">
+        <f>"https://doi.org/" &amp; D17</f>
         <v>https://doi.org/10.1016/j.compstruct.2020.112861</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>17</v>
       </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
+      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18" t="b">
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
         <v>1</v>
       </c>
       <c r="N18" t="b">
         <v>1</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
         <v>171</v>
       </c>
-      <c r="P18" t="str">
-        <f>"\cite{" &amp;C18 &amp; "} &amp; " &amp; IF(E18,"\checkmark","") &amp; " &amp; "&amp; IF(F18,"\checkmark","") &amp; " &amp; "&amp; IF(G18,"\checkmark","") &amp; " &amp; "&amp; IF(H18,"\checkmark","") &amp; " &amp; "&amp; IF(I18,"\checkmark","") &amp; " &amp; "&amp; IF(J18,"\checkmark","") &amp; " &amp; "&amp; IF(K18,"\checkmark","") &amp; " &amp; "&amp; IF(L18,"\checkmark","") &amp; " &amp; "&amp; IF(M18,"\checkmark","") &amp; " &amp; "&amp; IF(N18,"\checkmark","") &amp; " \\"</f>
+      <c r="R18" t="str">
+        <f>"\cite{" &amp;E18 &amp; "} &amp; " &amp; IF(G18,"\checkmark","") &amp; " &amp; "&amp; IF(H18,"\checkmark","") &amp; " &amp; "&amp; IF(I18,"\checkmark","") &amp; " &amp; "&amp; IF(J18,"\checkmark","") &amp; " &amp; "&amp; IF(K18,"\checkmark","") &amp; " &amp; "&amp; IF(L18,"\checkmark","") &amp; " &amp; "&amp; IF(M18,"\checkmark","") &amp; " &amp; "&amp; IF(N18,"\checkmark","") &amp; " &amp; "&amp; IF(O18,"\checkmark","") &amp; " &amp; "&amp; IF(P18,"\checkmark","") &amp; " \\"</f>
         <v>\cite{willmann_health_2023} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE18" t="str">
-        <f>"https://doi.org/" &amp; B18</f>
+      <c r="AG18" t="str">
+        <f>"https://doi.org/" &amp; D18</f>
         <v>https://doi.org/10.1016/j.compstruct.2023.116696</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>55</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>18</v>
       </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
       <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
       </c>
-      <c r="L19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" t="b">
+      <c r="K19" t="b">
         <v>1</v>
       </c>
       <c r="N19" t="b">
         <v>1</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
         <v>172</v>
       </c>
-      <c r="P19" t="str">
-        <f>"\cite{" &amp;C19 &amp; "} &amp; " &amp; IF(E19,"\checkmark","") &amp; " &amp; "&amp; IF(F19,"\checkmark","") &amp; " &amp; "&amp; IF(G19,"\checkmark","") &amp; " &amp; "&amp; IF(H19,"\checkmark","") &amp; " &amp; "&amp; IF(I19,"\checkmark","") &amp; " &amp; "&amp; IF(J19,"\checkmark","") &amp; " &amp; "&amp; IF(K19,"\checkmark","") &amp; " &amp; "&amp; IF(L19,"\checkmark","") &amp; " &amp; "&amp; IF(M19,"\checkmark","") &amp; " &amp; "&amp; IF(N19,"\checkmark","") &amp; " \\"</f>
+      <c r="R19" t="str">
+        <f>"\cite{" &amp;E19 &amp; "} &amp; " &amp; IF(G19,"\checkmark","") &amp; " &amp; "&amp; IF(H19,"\checkmark","") &amp; " &amp; "&amp; IF(I19,"\checkmark","") &amp; " &amp; "&amp; IF(J19,"\checkmark","") &amp; " &amp; "&amp; IF(K19,"\checkmark","") &amp; " &amp; "&amp; IF(L19,"\checkmark","") &amp; " &amp; "&amp; IF(M19,"\checkmark","") &amp; " &amp; "&amp; IF(N19,"\checkmark","") &amp; " &amp; "&amp; IF(O19,"\checkmark","") &amp; " &amp; "&amp; IF(P19,"\checkmark","") &amp; " \\"</f>
         <v>\cite{tang_explainable_2023} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE19" t="str">
-        <f>"https://doi.org/" &amp; B19</f>
+      <c r="AG19" t="str">
+        <f>"https://doi.org/" &amp; D19</f>
         <v>https://doi.org/10.1016/j.measurement.2022.112277</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>57</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>19</v>
       </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
       </c>
-      <c r="M20" t="b">
-        <v>1</v>
-      </c>
-      <c r="O20" t="s">
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
         <v>173</v>
       </c>
-      <c r="P20" t="str">
-        <f>"\cite{" &amp;C20 &amp; "} &amp; " &amp; IF(E20,"\checkmark","") &amp; " &amp; "&amp; IF(F20,"\checkmark","") &amp; " &amp; "&amp; IF(G20,"\checkmark","") &amp; " &amp; "&amp; IF(H20,"\checkmark","") &amp; " &amp; "&amp; IF(I20,"\checkmark","") &amp; " &amp; "&amp; IF(J20,"\checkmark","") &amp; " &amp; "&amp; IF(K20,"\checkmark","") &amp; " &amp; "&amp; IF(L20,"\checkmark","") &amp; " &amp; "&amp; IF(M20,"\checkmark","") &amp; " &amp; "&amp; IF(N20,"\checkmark","") &amp; " \\"</f>
+      <c r="R20" t="str">
+        <f>"\cite{" &amp;E20 &amp; "} &amp; " &amp; IF(G20,"\checkmark","") &amp; " &amp; "&amp; IF(H20,"\checkmark","") &amp; " &amp; "&amp; IF(I20,"\checkmark","") &amp; " &amp; "&amp; IF(J20,"\checkmark","") &amp; " &amp; "&amp; IF(K20,"\checkmark","") &amp; " &amp; "&amp; IF(L20,"\checkmark","") &amp; " &amp; "&amp; IF(M20,"\checkmark","") &amp; " &amp; "&amp; IF(N20,"\checkmark","") &amp; " &amp; "&amp; IF(O20,"\checkmark","") &amp; " &amp; "&amp; IF(P20,"\checkmark","") &amp; " \\"</f>
         <v>\cite{dong_ultrasonic_2022} &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE20" t="str">
-        <f>"https://doi.org/" &amp; B20</f>
+      <c r="AG20" t="str">
+        <f>"https://doi.org/" &amp; D20</f>
         <v>https://doi.org/10.1016/j.sna.2022.113528</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>56</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>20</v>
       </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
         <v>174</v>
       </c>
-      <c r="P21" t="str">
-        <f>"\cite{" &amp;C21 &amp; "} &amp; " &amp; IF(E21,"\checkmark","") &amp; " &amp; "&amp; IF(F21,"\checkmark","") &amp; " &amp; "&amp; IF(G21,"\checkmark","") &amp; " &amp; "&amp; IF(H21,"\checkmark","") &amp; " &amp; "&amp; IF(I21,"\checkmark","") &amp; " &amp; "&amp; IF(J21,"\checkmark","") &amp; " &amp; "&amp; IF(K21,"\checkmark","") &amp; " &amp; "&amp; IF(L21,"\checkmark","") &amp; " &amp; "&amp; IF(M21,"\checkmark","") &amp; " &amp; "&amp; IF(N21,"\checkmark","") &amp; " \\"</f>
+      <c r="R21" t="str">
+        <f>"\cite{" &amp;E21 &amp; "} &amp; " &amp; IF(G21,"\checkmark","") &amp; " &amp; "&amp; IF(H21,"\checkmark","") &amp; " &amp; "&amp; IF(I21,"\checkmark","") &amp; " &amp; "&amp; IF(J21,"\checkmark","") &amp; " &amp; "&amp; IF(K21,"\checkmark","") &amp; " &amp; "&amp; IF(L21,"\checkmark","") &amp; " &amp; "&amp; IF(M21,"\checkmark","") &amp; " &amp; "&amp; IF(N21,"\checkmark","") &amp; " &amp; "&amp; IF(O21,"\checkmark","") &amp; " &amp; "&amp; IF(P21,"\checkmark","") &amp; " \\"</f>
         <v>\cite{pachon_evaluation_2020} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE21" t="str">
-        <f>"https://doi.org/" &amp; B21</f>
+      <c r="AG21" t="str">
+        <f>"https://doi.org/" &amp; D21</f>
         <v>https://doi.org/10.1016/j.engstruct.2019.109843</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>58</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>21</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="b">
+      <c r="G22" t="b">
         <v>1</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
       </c>
-      <c r="K22" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22" t="b">
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
         <v>1</v>
       </c>
       <c r="N22" t="b">
         <v>1</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
         <v>175</v>
       </c>
-      <c r="P22" t="str">
-        <f>"\cite{" &amp;C22 &amp; "} &amp; " &amp; IF(E22,"\checkmark","") &amp; " &amp; "&amp; IF(F22,"\checkmark","") &amp; " &amp; "&amp; IF(G22,"\checkmark","") &amp; " &amp; "&amp; IF(H22,"\checkmark","") &amp; " &amp; "&amp; IF(I22,"\checkmark","") &amp; " &amp; "&amp; IF(J22,"\checkmark","") &amp; " &amp; "&amp; IF(K22,"\checkmark","") &amp; " &amp; "&amp; IF(L22,"\checkmark","") &amp; " &amp; "&amp; IF(M22,"\checkmark","") &amp; " &amp; "&amp; IF(N22,"\checkmark","") &amp; " \\"</f>
+      <c r="R22" t="str">
+        <f>"\cite{" &amp;E22 &amp; "} &amp; " &amp; IF(G22,"\checkmark","") &amp; " &amp; "&amp; IF(H22,"\checkmark","") &amp; " &amp; "&amp; IF(I22,"\checkmark","") &amp; " &amp; "&amp; IF(J22,"\checkmark","") &amp; " &amp; "&amp; IF(K22,"\checkmark","") &amp; " &amp; "&amp; IF(L22,"\checkmark","") &amp; " &amp; "&amp; IF(M22,"\checkmark","") &amp; " &amp; "&amp; IF(N22,"\checkmark","") &amp; " &amp; "&amp; IF(O22,"\checkmark","") &amp; " &amp; "&amp; IF(P22,"\checkmark","") &amp; " \\"</f>
         <v>\cite{de_sa_rodrigues_probability_2023} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE22" t="str">
-        <f>"https://doi.org/" &amp; B22</f>
+      <c r="AG22" t="str">
+        <f>"https://doi.org/" &amp; D22</f>
         <v>https://doi.org/10.1016/j.ndteint.2023.102924</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>59</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>22</v>
       </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" t="b">
+      <c r="K23" t="b">
         <v>1</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
       </c>
-      <c r="M23" t="b">
-        <v>1</v>
-      </c>
       <c r="N23" t="b">
         <v>1</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
         <v>176</v>
       </c>
-      <c r="P23" t="str">
-        <f>"\cite{" &amp;C23 &amp; "} &amp; " &amp; IF(E23,"\checkmark","") &amp; " &amp; "&amp; IF(F23,"\checkmark","") &amp; " &amp; "&amp; IF(G23,"\checkmark","") &amp; " &amp; "&amp; IF(H23,"\checkmark","") &amp; " &amp; "&amp; IF(I23,"\checkmark","") &amp; " &amp; "&amp; IF(J23,"\checkmark","") &amp; " &amp; "&amp; IF(K23,"\checkmark","") &amp; " &amp; "&amp; IF(L23,"\checkmark","") &amp; " &amp; "&amp; IF(M23,"\checkmark","") &amp; " &amp; "&amp; IF(N23,"\checkmark","") &amp; " \\"</f>
+      <c r="R23" t="str">
+        <f>"\cite{" &amp;E23 &amp; "} &amp; " &amp; IF(G23,"\checkmark","") &amp; " &amp; "&amp; IF(H23,"\checkmark","") &amp; " &amp; "&amp; IF(I23,"\checkmark","") &amp; " &amp; "&amp; IF(J23,"\checkmark","") &amp; " &amp; "&amp; IF(K23,"\checkmark","") &amp; " &amp; "&amp; IF(L23,"\checkmark","") &amp; " &amp; "&amp; IF(M23,"\checkmark","") &amp; " &amp; "&amp; IF(N23,"\checkmark","") &amp; " &amp; "&amp; IF(O23,"\checkmark","") &amp; " &amp; "&amp; IF(P23,"\checkmark","") &amp; " \\"</f>
         <v>\cite{wu_internal_2024} &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE23" t="str">
-        <f>"https://doi.org/" &amp; B23</f>
+      <c r="AG23" t="str">
+        <f>"https://doi.org/" &amp; D23</f>
         <v>https://doi.org/10.1016/j.measurement.2024.114262</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>60</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>23</v>
       </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
+      <c r="G24" t="b">
         <v>1</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
       </c>
-      <c r="M24" t="b">
-        <v>1</v>
-      </c>
-      <c r="N24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O24" t="s">
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
         <v>177</v>
       </c>
-      <c r="P24" t="str">
-        <f>"\cite{" &amp;C24 &amp; "} &amp; " &amp; IF(E24,"\checkmark","") &amp; " &amp; "&amp; IF(F24,"\checkmark","") &amp; " &amp; "&amp; IF(G24,"\checkmark","") &amp; " &amp; "&amp; IF(H24,"\checkmark","") &amp; " &amp; "&amp; IF(I24,"\checkmark","") &amp; " &amp; "&amp; IF(J24,"\checkmark","") &amp; " &amp; "&amp; IF(K24,"\checkmark","") &amp; " &amp; "&amp; IF(L24,"\checkmark","") &amp; " &amp; "&amp; IF(M24,"\checkmark","") &amp; " &amp; "&amp; IF(N24,"\checkmark","") &amp; " \\"</f>
+      <c r="R24" t="str">
+        <f>"\cite{" &amp;E24 &amp; "} &amp; " &amp; IF(G24,"\checkmark","") &amp; " &amp; "&amp; IF(H24,"\checkmark","") &amp; " &amp; "&amp; IF(I24,"\checkmark","") &amp; " &amp; "&amp; IF(J24,"\checkmark","") &amp; " &amp; "&amp; IF(K24,"\checkmark","") &amp; " &amp; "&amp; IF(L24,"\checkmark","") &amp; " &amp; "&amp; IF(M24,"\checkmark","") &amp; " &amp; "&amp; IF(N24,"\checkmark","") &amp; " &amp; "&amp; IF(O24,"\checkmark","") &amp; " &amp; "&amp; IF(P24,"\checkmark","") &amp; " \\"</f>
         <v>\cite{fang_structural_2024} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp;  &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE24" t="str">
-        <f>"https://doi.org/" &amp; B24</f>
+      <c r="AG24" t="str">
+        <f>"https://doi.org/" &amp; D24</f>
         <v>https://doi.org/10.1016/j.measurement.2023.114023</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>61</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>24</v>
       </c>
-      <c r="G25" t="b">
-        <v>1</v>
-      </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
       </c>
-      <c r="L25" t="b">
-        <v>1</v>
-      </c>
       <c r="M25" t="b">
         <v>1</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
         <v>178</v>
       </c>
-      <c r="P25" t="str">
-        <f>"\cite{" &amp;C25 &amp; "} &amp; " &amp; IF(E25,"\checkmark","") &amp; " &amp; "&amp; IF(F25,"\checkmark","") &amp; " &amp; "&amp; IF(G25,"\checkmark","") &amp; " &amp; "&amp; IF(H25,"\checkmark","") &amp; " &amp; "&amp; IF(I25,"\checkmark","") &amp; " &amp; "&amp; IF(J25,"\checkmark","") &amp; " &amp; "&amp; IF(K25,"\checkmark","") &amp; " &amp; "&amp; IF(L25,"\checkmark","") &amp; " &amp; "&amp; IF(M25,"\checkmark","") &amp; " &amp; "&amp; IF(N25,"\checkmark","") &amp; " \\"</f>
+      <c r="R25" t="str">
+        <f>"\cite{" &amp;E25 &amp; "} &amp; " &amp; IF(G25,"\checkmark","") &amp; " &amp; "&amp; IF(H25,"\checkmark","") &amp; " &amp; "&amp; IF(I25,"\checkmark","") &amp; " &amp; "&amp; IF(J25,"\checkmark","") &amp; " &amp; "&amp; IF(K25,"\checkmark","") &amp; " &amp; "&amp; IF(L25,"\checkmark","") &amp; " &amp; "&amp; IF(M25,"\checkmark","") &amp; " &amp; "&amp; IF(N25,"\checkmark","") &amp; " &amp; "&amp; IF(O25,"\checkmark","") &amp; " &amp; "&amp; IF(P25,"\checkmark","") &amp; " \\"</f>
         <v>\cite{meng_effects_2021} &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE25" t="str">
-        <f>"https://doi.org/" &amp; B25</f>
+      <c r="AG25" t="str">
+        <f>"https://doi.org/" &amp; D25</f>
         <v>https://doi.org/10.1016/j.measurement.2021.109708</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>62</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>25</v>
       </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
       <c r="H26" t="b">
         <v>1</v>
       </c>
@@ -2072,121 +2222,139 @@
       <c r="N26" t="b">
         <v>1</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
         <v>179</v>
       </c>
-      <c r="P26" t="str">
-        <f>"\cite{" &amp;C26 &amp; "} &amp; " &amp; IF(E26,"\checkmark","") &amp; " &amp; "&amp; IF(F26,"\checkmark","") &amp; " &amp; "&amp; IF(G26,"\checkmark","") &amp; " &amp; "&amp; IF(H26,"\checkmark","") &amp; " &amp; "&amp; IF(I26,"\checkmark","") &amp; " &amp; "&amp; IF(J26,"\checkmark","") &amp; " &amp; "&amp; IF(K26,"\checkmark","") &amp; " &amp; "&amp; IF(L26,"\checkmark","") &amp; " &amp; "&amp; IF(M26,"\checkmark","") &amp; " &amp; "&amp; IF(N26,"\checkmark","") &amp; " \\"</f>
+      <c r="R26" t="str">
+        <f>"\cite{" &amp;E26 &amp; "} &amp; " &amp; IF(G26,"\checkmark","") &amp; " &amp; "&amp; IF(H26,"\checkmark","") &amp; " &amp; "&amp; IF(I26,"\checkmark","") &amp; " &amp; "&amp; IF(J26,"\checkmark","") &amp; " &amp; "&amp; IF(K26,"\checkmark","") &amp; " &amp; "&amp; IF(L26,"\checkmark","") &amp; " &amp; "&amp; IF(M26,"\checkmark","") &amp; " &amp; "&amp; IF(N26,"\checkmark","") &amp; " &amp; "&amp; IF(O26,"\checkmark","") &amp; " &amp; "&amp; IF(P26,"\checkmark","") &amp; " \\"</f>
         <v>\cite{katunin_identification_2021} &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE26" t="str">
-        <f>"https://doi.org/" &amp; B26</f>
+      <c r="AG26" t="str">
+        <f>"https://doi.org/" &amp; D26</f>
         <v>https://doi.org/10.1016/j.measurement.2020.108656</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
         <v>27</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>63</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>26</v>
       </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
       </c>
-      <c r="L27" t="b">
+      <c r="K27" t="b">
         <v>1</v>
       </c>
       <c r="N27" t="b">
         <v>1</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
         <v>180</v>
       </c>
-      <c r="P27" t="str">
-        <f>"\cite{" &amp;C27 &amp; "} &amp; " &amp; IF(E27,"\checkmark","") &amp; " &amp; "&amp; IF(F27,"\checkmark","") &amp; " &amp; "&amp; IF(G27,"\checkmark","") &amp; " &amp; "&amp; IF(H27,"\checkmark","") &amp; " &amp; "&amp; IF(I27,"\checkmark","") &amp; " &amp; "&amp; IF(J27,"\checkmark","") &amp; " &amp; "&amp; IF(K27,"\checkmark","") &amp; " &amp; "&amp; IF(L27,"\checkmark","") &amp; " &amp; "&amp; IF(M27,"\checkmark","") &amp; " &amp; "&amp; IF(N27,"\checkmark","") &amp; " \\"</f>
+      <c r="R27" t="str">
+        <f>"\cite{" &amp;E27 &amp; "} &amp; " &amp; IF(G27,"\checkmark","") &amp; " &amp; "&amp; IF(H27,"\checkmark","") &amp; " &amp; "&amp; IF(I27,"\checkmark","") &amp; " &amp; "&amp; IF(J27,"\checkmark","") &amp; " &amp; "&amp; IF(K27,"\checkmark","") &amp; " &amp; "&amp; IF(L27,"\checkmark","") &amp; " &amp; "&amp; IF(M27,"\checkmark","") &amp; " &amp; "&amp; IF(N27,"\checkmark","") &amp; " &amp; "&amp; IF(O27,"\checkmark","") &amp; " &amp; "&amp; IF(P27,"\checkmark","") &amp; " \\"</f>
         <v>\cite{de_menezes_defect_2021} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE27" t="str">
-        <f>"https://doi.org/" &amp; B27</f>
+      <c r="AG27" t="str">
+        <f>"https://doi.org/" &amp; D27</f>
         <v>https://doi.org/10.1016/j.compstruct.2021.114548</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
         <v>28</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>64</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>27</v>
       </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
+      <c r="G28" t="b">
         <v>1</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
       </c>
-      <c r="K28" t="b">
-        <v>1</v>
-      </c>
-      <c r="L28" t="b">
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
         <v>1</v>
       </c>
       <c r="N28" t="b">
         <v>1</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="s">
         <v>181</v>
       </c>
-      <c r="P28" t="str">
-        <f>"\cite{" &amp;C28 &amp; "} &amp; " &amp; IF(E28,"\checkmark","") &amp; " &amp; "&amp; IF(F28,"\checkmark","") &amp; " &amp; "&amp; IF(G28,"\checkmark","") &amp; " &amp; "&amp; IF(H28,"\checkmark","") &amp; " &amp; "&amp; IF(I28,"\checkmark","") &amp; " &amp; "&amp; IF(J28,"\checkmark","") &amp; " &amp; "&amp; IF(K28,"\checkmark","") &amp; " &amp; "&amp; IF(L28,"\checkmark","") &amp; " &amp; "&amp; IF(M28,"\checkmark","") &amp; " &amp; "&amp; IF(N28,"\checkmark","") &amp; " \\"</f>
+      <c r="R28" t="str">
+        <f>"\cite{" &amp;E28 &amp; "} &amp; " &amp; IF(G28,"\checkmark","") &amp; " &amp; "&amp; IF(H28,"\checkmark","") &amp; " &amp; "&amp; IF(I28,"\checkmark","") &amp; " &amp; "&amp; IF(J28,"\checkmark","") &amp; " &amp; "&amp; IF(K28,"\checkmark","") &amp; " &amp; "&amp; IF(L28,"\checkmark","") &amp; " &amp; "&amp; IF(M28,"\checkmark","") &amp; " &amp; "&amp; IF(N28,"\checkmark","") &amp; " &amp; "&amp; IF(O28,"\checkmark","") &amp; " &amp; "&amp; IF(P28,"\checkmark","") &amp; " \\"</f>
         <v>\cite{zhang_structural_2021} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE28" t="str">
-        <f>"https://doi.org/" &amp; B28</f>
+      <c r="AG28" t="str">
+        <f>"https://doi.org/" &amp; D28</f>
         <v>https://doi.org/10.1016/j.measurement.2020.108343</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
         <v>29</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>65</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>28</v>
       </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
       <c r="I29" t="b">
         <v>1</v>
       </c>
-      <c r="J29" t="b">
+      <c r="K29" t="b">
         <v>1</v>
       </c>
       <c r="L29" t="b">
@@ -2195,117 +2363,135 @@
       <c r="N29" t="b">
         <v>1</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="s">
         <v>182</v>
       </c>
-      <c r="P29" t="str">
-        <f>"\cite{" &amp;C29 &amp; "} &amp; " &amp; IF(E29,"\checkmark","") &amp; " &amp; "&amp; IF(F29,"\checkmark","") &amp; " &amp; "&amp; IF(G29,"\checkmark","") &amp; " &amp; "&amp; IF(H29,"\checkmark","") &amp; " &amp; "&amp; IF(I29,"\checkmark","") &amp; " &amp; "&amp; IF(J29,"\checkmark","") &amp; " &amp; "&amp; IF(K29,"\checkmark","") &amp; " &amp; "&amp; IF(L29,"\checkmark","") &amp; " &amp; "&amp; IF(M29,"\checkmark","") &amp; " &amp; "&amp; IF(N29,"\checkmark","") &amp; " \\"</f>
+      <c r="R29" t="str">
+        <f>"\cite{" &amp;E29 &amp; "} &amp; " &amp; IF(G29,"\checkmark","") &amp; " &amp; "&amp; IF(H29,"\checkmark","") &amp; " &amp; "&amp; IF(I29,"\checkmark","") &amp; " &amp; "&amp; IF(J29,"\checkmark","") &amp; " &amp; "&amp; IF(K29,"\checkmark","") &amp; " &amp; "&amp; IF(L29,"\checkmark","") &amp; " &amp; "&amp; IF(M29,"\checkmark","") &amp; " &amp; "&amp; IF(N29,"\checkmark","") &amp; " &amp; "&amp; IF(O29,"\checkmark","") &amp; " &amp; "&amp; IF(P29,"\checkmark","") &amp; " \\"</f>
         <v>\cite{li_physics-informed_2023} &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE29" t="str">
-        <f>"https://doi.org/" &amp; B29</f>
+      <c r="AG29" t="str">
+        <f>"https://doi.org/" &amp; D29</f>
         <v>https://doi.org/10.1016/j.jsv.2023.118066</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
         <v>30</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>66</v>
       </c>
-      <c r="D30">
+      <c r="F30">
         <v>29</v>
       </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="b">
+      <c r="G30" t="b">
         <v>1</v>
       </c>
       <c r="H30" t="b">
         <v>1</v>
       </c>
-      <c r="L30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M30" t="b">
+      <c r="J30" t="b">
         <v>1</v>
       </c>
       <c r="N30" t="b">
         <v>1</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
         <v>183</v>
       </c>
-      <c r="P30" t="str">
-        <f>"\cite{" &amp;C30 &amp; "} &amp; " &amp; IF(E30,"\checkmark","") &amp; " &amp; "&amp; IF(F30,"\checkmark","") &amp; " &amp; "&amp; IF(G30,"\checkmark","") &amp; " &amp; "&amp; IF(H30,"\checkmark","") &amp; " &amp; "&amp; IF(I30,"\checkmark","") &amp; " &amp; "&amp; IF(J30,"\checkmark","") &amp; " &amp; "&amp; IF(K30,"\checkmark","") &amp; " &amp; "&amp; IF(L30,"\checkmark","") &amp; " &amp; "&amp; IF(M30,"\checkmark","") &amp; " &amp; "&amp; IF(N30,"\checkmark","") &amp; " \\"</f>
+      <c r="R30" t="str">
+        <f>"\cite{" &amp;E30 &amp; "} &amp; " &amp; IF(G30,"\checkmark","") &amp; " &amp; "&amp; IF(H30,"\checkmark","") &amp; " &amp; "&amp; IF(I30,"\checkmark","") &amp; " &amp; "&amp; IF(J30,"\checkmark","") &amp; " &amp; "&amp; IF(K30,"\checkmark","") &amp; " &amp; "&amp; IF(L30,"\checkmark","") &amp; " &amp; "&amp; IF(M30,"\checkmark","") &amp; " &amp; "&amp; IF(N30,"\checkmark","") &amp; " &amp; "&amp; IF(O30,"\checkmark","") &amp; " &amp; "&amp; IF(P30,"\checkmark","") &amp; " \\"</f>
         <v>\cite{zhang_defect_2020} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE30" t="str">
-        <f>"https://doi.org/" &amp; B30</f>
+      <c r="AG30" t="str">
+        <f>"https://doi.org/" &amp; D30</f>
         <v>https://doi.org/10.1016/j.measurement.2019.107280</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>67</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>30</v>
       </c>
-      <c r="G31" t="b">
-        <v>1</v>
-      </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="K31" t="b">
         <v>1</v>
       </c>
-      <c r="L31" t="b">
+      <c r="M31" t="b">
         <v>1</v>
       </c>
       <c r="N31" t="b">
         <v>1</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
         <v>184</v>
       </c>
-      <c r="P31" t="str">
-        <f>"\cite{" &amp;C31 &amp; "} &amp; " &amp; IF(E31,"\checkmark","") &amp; " &amp; "&amp; IF(F31,"\checkmark","") &amp; " &amp; "&amp; IF(G31,"\checkmark","") &amp; " &amp; "&amp; IF(H31,"\checkmark","") &amp; " &amp; "&amp; IF(I31,"\checkmark","") &amp; " &amp; "&amp; IF(J31,"\checkmark","") &amp; " &amp; "&amp; IF(K31,"\checkmark","") &amp; " &amp; "&amp; IF(L31,"\checkmark","") &amp; " &amp; "&amp; IF(M31,"\checkmark","") &amp; " &amp; "&amp; IF(N31,"\checkmark","") &amp; " \\"</f>
+      <c r="R31" t="str">
+        <f>"\cite{" &amp;E31 &amp; "} &amp; " &amp; IF(G31,"\checkmark","") &amp; " &amp; "&amp; IF(H31,"\checkmark","") &amp; " &amp; "&amp; IF(I31,"\checkmark","") &amp; " &amp; "&amp; IF(J31,"\checkmark","") &amp; " &amp; "&amp; IF(K31,"\checkmark","") &amp; " &amp; "&amp; IF(L31,"\checkmark","") &amp; " &amp; "&amp; IF(M31,"\checkmark","") &amp; " &amp; "&amp; IF(N31,"\checkmark","") &amp; " &amp; "&amp; IF(O31,"\checkmark","") &amp; " &amp; "&amp; IF(P31,"\checkmark","") &amp; " \\"</f>
         <v>\cite{zima_damage_2021} &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark \\</v>
       </c>
-      <c r="AE31" t="str">
-        <f>"https://doi.org/" &amp; B31</f>
+      <c r="AG31" t="str">
+        <f>"https://doi.org/" &amp; D31</f>
         <v>https://doi.org/10.1016/j.measurement.2021.109206</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>68</v>
       </c>
-      <c r="D32">
+      <c r="F32">
         <v>31</v>
       </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
       <c r="H32" t="b">
         <v>1</v>
       </c>
@@ -2315,87 +2501,96 @@
       <c r="L32" t="b">
         <v>1</v>
       </c>
-      <c r="M32" t="b">
-        <v>1</v>
-      </c>
-      <c r="O32" t="s">
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
         <v>185</v>
       </c>
-      <c r="P32" t="str">
-        <f>"\cite{" &amp;C32 &amp; "} &amp; " &amp; IF(E32,"\checkmark","") &amp; " &amp; "&amp; IF(F32,"\checkmark","") &amp; " &amp; "&amp; IF(G32,"\checkmark","") &amp; " &amp; "&amp; IF(H32,"\checkmark","") &amp; " &amp; "&amp; IF(I32,"\checkmark","") &amp; " &amp; "&amp; IF(J32,"\checkmark","") &amp; " &amp; "&amp; IF(K32,"\checkmark","") &amp; " &amp; "&amp; IF(L32,"\checkmark","") &amp; " &amp; "&amp; IF(M32,"\checkmark","") &amp; " &amp; "&amp; IF(N32,"\checkmark","") &amp; " \\"</f>
+      <c r="R32" t="str">
+        <f>"\cite{" &amp;E32 &amp; "} &amp; " &amp; IF(G32,"\checkmark","") &amp; " &amp; "&amp; IF(H32,"\checkmark","") &amp; " &amp; "&amp; IF(I32,"\checkmark","") &amp; " &amp; "&amp; IF(J32,"\checkmark","") &amp; " &amp; "&amp; IF(K32,"\checkmark","") &amp; " &amp; "&amp; IF(L32,"\checkmark","") &amp; " &amp; "&amp; IF(M32,"\checkmark","") &amp; " &amp; "&amp; IF(N32,"\checkmark","") &amp; " &amp; "&amp; IF(O32,"\checkmark","") &amp; " &amp; "&amp; IF(P32,"\checkmark","") &amp; " \\"</f>
         <v>\cite{wang_fatigue_2023} &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE32" t="str">
-        <f>"https://doi.org/" &amp; B32</f>
+      <c r="AG32" t="str">
+        <f>"https://doi.org/" &amp; D32</f>
         <v>https://doi.org/10.1016/j.compstruct.2023.117239</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>69</v>
       </c>
-      <c r="D33">
+      <c r="F33">
         <v>32</v>
       </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
       <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
-      <c r="M33" t="b">
-        <v>1</v>
-      </c>
-      <c r="N33" t="b">
-        <v>1</v>
-      </c>
-      <c r="O33" t="s">
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
         <v>186</v>
       </c>
-      <c r="P33" t="str">
-        <f>"\cite{" &amp;C33 &amp; "} &amp; " &amp; IF(E33,"\checkmark","") &amp; " &amp; "&amp; IF(F33,"\checkmark","") &amp; " &amp; "&amp; IF(G33,"\checkmark","") &amp; " &amp; "&amp; IF(H33,"\checkmark","") &amp; " &amp; "&amp; IF(I33,"\checkmark","") &amp; " &amp; "&amp; IF(J33,"\checkmark","") &amp; " &amp; "&amp; IF(K33,"\checkmark","") &amp; " &amp; "&amp; IF(L33,"\checkmark","") &amp; " &amp; "&amp; IF(M33,"\checkmark","") &amp; " &amp; "&amp; IF(N33,"\checkmark","") &amp; " \\"</f>
+      <c r="R33" t="str">
+        <f>"\cite{" &amp;E33 &amp; "} &amp; " &amp; IF(G33,"\checkmark","") &amp; " &amp; "&amp; IF(H33,"\checkmark","") &amp; " &amp; "&amp; IF(I33,"\checkmark","") &amp; " &amp; "&amp; IF(J33,"\checkmark","") &amp; " &amp; "&amp; IF(K33,"\checkmark","") &amp; " &amp; "&amp; IF(L33,"\checkmark","") &amp; " &amp; "&amp; IF(M33,"\checkmark","") &amp; " &amp; "&amp; IF(N33,"\checkmark","") &amp; " &amp; "&amp; IF(O33,"\checkmark","") &amp; " &amp; "&amp; IF(P33,"\checkmark","") &amp; " \\"</f>
         <v>\cite{han_crack_2021} &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE33" t="str">
-        <f>"https://doi.org/" &amp; B33</f>
+      <c r="AG33" t="str">
+        <f>"https://doi.org/" &amp; D33</f>
         <v>https://doi.org/10.1016/j.measurement.2021.109461</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34">
         <v>34</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" t="s">
         <v>70</v>
       </c>
-      <c r="D34">
+      <c r="F34">
         <v>33</v>
       </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
+      <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="H34" t="b">
         <v>1</v>
       </c>
-      <c r="K34" t="b">
-        <v>1</v>
-      </c>
-      <c r="L34" t="b">
+      <c r="J34" t="b">
         <v>1</v>
       </c>
       <c r="M34" t="b">
@@ -2404,108 +2599,119 @@
       <c r="N34" t="b">
         <v>1</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="s">
         <v>187</v>
       </c>
-      <c r="P34" t="str">
-        <f>"\cite{" &amp;C34 &amp; "} &amp; " &amp; IF(E34,"\checkmark","") &amp; " &amp; "&amp; IF(F34,"\checkmark","") &amp; " &amp; "&amp; IF(G34,"\checkmark","") &amp; " &amp; "&amp; IF(H34,"\checkmark","") &amp; " &amp; "&amp; IF(I34,"\checkmark","") &amp; " &amp; "&amp; IF(J34,"\checkmark","") &amp; " &amp; "&amp; IF(K34,"\checkmark","") &amp; " &amp; "&amp; IF(L34,"\checkmark","") &amp; " &amp; "&amp; IF(M34,"\checkmark","") &amp; " &amp; "&amp; IF(N34,"\checkmark","") &amp; " \\"</f>
+      <c r="R34" t="str">
+        <f>"\cite{" &amp;E34 &amp; "} &amp; " &amp; IF(G34,"\checkmark","") &amp; " &amp; "&amp; IF(H34,"\checkmark","") &amp; " &amp; "&amp; IF(I34,"\checkmark","") &amp; " &amp; "&amp; IF(J34,"\checkmark","") &amp; " &amp; "&amp; IF(K34,"\checkmark","") &amp; " &amp; "&amp; IF(L34,"\checkmark","") &amp; " &amp; "&amp; IF(M34,"\checkmark","") &amp; " &amp; "&amp; IF(N34,"\checkmark","") &amp; " &amp; "&amp; IF(O34,"\checkmark","") &amp; " &amp; "&amp; IF(P34,"\checkmark","") &amp; " \\"</f>
         <v>\cite{yifei_structure_2023} &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp; \checkmark &amp; \checkmark \\</v>
       </c>
-      <c r="AE34" t="str">
-        <f>"https://doi.org/" &amp; B34</f>
+      <c r="AG34" t="str">
+        <f>"https://doi.org/" &amp; D34</f>
         <v>https://doi.org/10.1016/j.engstruct.2023.115891</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>71</v>
       </c>
-      <c r="D35">
+      <c r="F35">
         <v>34</v>
       </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
       <c r="I35" t="b">
         <v>1</v>
       </c>
-      <c r="J35" t="b">
+      <c r="K35" t="b">
         <v>1</v>
       </c>
       <c r="L35" t="b">
         <v>1</v>
       </c>
-      <c r="M35" t="b">
-        <v>1</v>
-      </c>
-      <c r="O35" t="s">
+      <c r="N35" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
         <v>188</v>
       </c>
-      <c r="P35" t="str">
-        <f>"\cite{" &amp;C35 &amp; "} &amp; " &amp; IF(E35,"\checkmark","") &amp; " &amp; "&amp; IF(F35,"\checkmark","") &amp; " &amp; "&amp; IF(G35,"\checkmark","") &amp; " &amp; "&amp; IF(H35,"\checkmark","") &amp; " &amp; "&amp; IF(I35,"\checkmark","") &amp; " &amp; "&amp; IF(J35,"\checkmark","") &amp; " &amp; "&amp; IF(K35,"\checkmark","") &amp; " &amp; "&amp; IF(L35,"\checkmark","") &amp; " &amp; "&amp; IF(M35,"\checkmark","") &amp; " &amp; "&amp; IF(N35,"\checkmark","") &amp; " \\"</f>
+      <c r="R35" t="str">
+        <f>"\cite{" &amp;E35 &amp; "} &amp; " &amp; IF(G35,"\checkmark","") &amp; " &amp; "&amp; IF(H35,"\checkmark","") &amp; " &amp; "&amp; IF(I35,"\checkmark","") &amp; " &amp; "&amp; IF(J35,"\checkmark","") &amp; " &amp; "&amp; IF(K35,"\checkmark","") &amp; " &amp; "&amp; IF(L35,"\checkmark","") &amp; " &amp; "&amp; IF(M35,"\checkmark","") &amp; " &amp; "&amp; IF(N35,"\checkmark","") &amp; " &amp; "&amp; IF(O35,"\checkmark","") &amp; " &amp; "&amp; IF(P35,"\checkmark","") &amp; " \\"</f>
         <v>\cite{bevan_automated_2022} &amp;  &amp;  &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE35" t="str">
-        <f>"https://doi.org/" &amp; B35</f>
+      <c r="AG35" t="str">
+        <f>"https://doi.org/" &amp; D35</f>
         <v>https://doi.org/10.1016/j.ndteint.2022.102628</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
         <v>36</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>72</v>
       </c>
-      <c r="D36">
+      <c r="F36">
         <v>35</v>
       </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="L36" t="b">
-        <v>1</v>
-      </c>
-      <c r="M36" t="b">
-        <v>1</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="s">
         <v>189</v>
       </c>
-      <c r="P36" t="str">
-        <f>"\cite{" &amp;C36 &amp; "} &amp; " &amp; IF(E36,"\checkmark","") &amp; " &amp; "&amp; IF(F36,"\checkmark","") &amp; " &amp; "&amp; IF(G36,"\checkmark","") &amp; " &amp; "&amp; IF(H36,"\checkmark","") &amp; " &amp; "&amp; IF(I36,"\checkmark","") &amp; " &amp; "&amp; IF(J36,"\checkmark","") &amp; " &amp; "&amp; IF(K36,"\checkmark","") &amp; " &amp; "&amp; IF(L36,"\checkmark","") &amp; " &amp; "&amp; IF(M36,"\checkmark","") &amp; " &amp; "&amp; IF(N36,"\checkmark","") &amp; " \\"</f>
+      <c r="R36" t="str">
+        <f>"\cite{" &amp;E36 &amp; "} &amp; " &amp; IF(G36,"\checkmark","") &amp; " &amp; "&amp; IF(H36,"\checkmark","") &amp; " &amp; "&amp; IF(I36,"\checkmark","") &amp; " &amp; "&amp; IF(J36,"\checkmark","") &amp; " &amp; "&amp; IF(K36,"\checkmark","") &amp; " &amp; "&amp; IF(L36,"\checkmark","") &amp; " &amp; "&amp; IF(M36,"\checkmark","") &amp; " &amp; "&amp; IF(N36,"\checkmark","") &amp; " &amp; "&amp; IF(O36,"\checkmark","") &amp; " &amp; "&amp; IF(P36,"\checkmark","") &amp; " \\"</f>
         <v>\cite{tabjula_sparse_2023} &amp;  &amp;  &amp; \checkmark &amp;  &amp;  &amp;  &amp;  &amp; \checkmark &amp; \checkmark &amp;  \\</v>
       </c>
-      <c r="AE36" t="str">
-        <f>"https://doi.org/" &amp; B36</f>
+      <c r="AG36" t="str">
+        <f>"https://doi.org/" &amp; D36</f>
         <v>https://doi.org/10.1016/j.ndteint.2023.102890</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG36">
     <sortCondition ref="A2:A36"/>
-    <sortCondition descending="1" ref="E2:E36"/>
-    <sortCondition descending="1" ref="F2:F36"/>
-    <sortCondition descending="1" ref="G2:G36"/>
-    <sortCondition descending="1" ref="H2:H36"/>
-    <sortCondition descending="1" ref="I2:I36"/>
-    <sortCondition descending="1" ref="J2:J36"/>
-    <sortCondition descending="1" ref="K2:K36"/>
-    <sortCondition descending="1" ref="L2:L36"/>
-    <sortCondition descending="1" ref="M2:M36"/>
-    <sortCondition descending="1" ref="N2:N36"/>
   </sortState>
-  <conditionalFormatting sqref="A1:C1048576 D1:O1">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <conditionalFormatting sqref="F1:Q1 A1:A1048576 C37:D1048576 D1:E36">
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B11 B2:B3 B13:B41">
+    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3648,8 +3854,8 @@
         <v>27</v>
       </c>
       <c r="I4" t="str">
-        <f>D4&amp;" \cite{"&amp;VLOOKUP(F4,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E4 &amp; " \\"</f>
-        <v>L. Zhang, et al. \cite{zhang_structural_2021} &amp; 111 \\</v>
+        <f>D4&amp;" \cite{"&amp;VLOOKUP(F4,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E4 &amp; " \\"</f>
+        <v>L. Zhang, et al. \cite{22} &amp; 111 \\</v>
       </c>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
@@ -3663,8 +3869,8 @@
         <v>29</v>
       </c>
       <c r="I5" t="str">
-        <f>D5&amp;" \cite{"&amp;VLOOKUP(F5,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E5 &amp; " \\"</f>
-        <v>W. Zhang, et al. \cite{zhang_defect_2020} &amp; 40 \\</v>
+        <f>D5&amp;" \cite{"&amp;VLOOKUP(F5,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E5 &amp; " \\"</f>
+        <v>W. Zhang, et al. \cite{24} &amp; 40 \\</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
@@ -3678,8 +3884,8 @@
         <v>16</v>
       </c>
       <c r="I6" t="str">
-        <f>D6&amp;" \cite{"&amp;VLOOKUP(F6,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E6 &amp; " \\"</f>
-        <v>O. Rufai et al. \cite{rufai_cure_2020} &amp; 36 \\</v>
+        <f>D6&amp;" \cite{"&amp;VLOOKUP(F6,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E6 &amp; " \\"</f>
+        <v>O. Rufai et al. \cite{13} &amp; 36 \\</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
@@ -3693,8 +3899,8 @@
         <v>20</v>
       </c>
       <c r="I7" t="str">
-        <f>D7&amp;" \cite{"&amp;VLOOKUP(F7,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E7 &amp; " \\"</f>
-        <v>P. Pachón et al \cite{pachon_evaluation_2020} &amp; 28 \\</v>
+        <f>D7&amp;" \cite{"&amp;VLOOKUP(F7,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E7 &amp; " \\"</f>
+        <v>P. Pachón et al \cite{17} &amp; 28 \\</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
@@ -3708,8 +3914,8 @@
         <v>10</v>
       </c>
       <c r="I8" t="str">
-        <f>D8&amp;" \cite{"&amp;VLOOKUP(F8,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E8 &amp; " \\"</f>
-        <v>F. Lambinet et al. \cite{lambinet_measurement_2022} &amp; 21 \\</v>
+        <f>D8&amp;" \cite{"&amp;VLOOKUP(F8,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E8 &amp; " \\"</f>
+        <v>F. Lambinet et al. \cite{8} &amp; 21 \\</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
@@ -3723,8 +3929,8 @@
         <v>33</v>
       </c>
       <c r="I9" t="str">
-        <f>D9&amp;" \cite{"&amp;VLOOKUP(F9,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E9 &amp; " \\"</f>
-        <v>L. YiFei et al. \cite{yifei_structure_2023} &amp; 21 \\</v>
+        <f>D9&amp;" \cite{"&amp;VLOOKUP(F9,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E9 &amp; " \\"</f>
+        <v>L. YiFei et al. \cite{28} &amp; 21 \\</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
@@ -3738,8 +3944,8 @@
         <v>7</v>
       </c>
       <c r="I10" t="str">
-        <f>D10&amp;" \cite{"&amp;VLOOKUP(F10,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E10 &amp; " \\"</f>
-        <v>A. Katunin, et al. \cite{katunin_modeling_2021} &amp; 17 \\</v>
+        <f>D10&amp;" \cite{"&amp;VLOOKUP(F10,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E10 &amp; " \\"</f>
+        <v>A. Katunin, et al. \cite{5} &amp; 17 \\</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
@@ -3753,8 +3959,8 @@
         <v>6</v>
       </c>
       <c r="I11" t="str">
-        <f>D11&amp;" \cite{"&amp;VLOOKUP(F11,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E11 &amp; " \\"</f>
-        <v>D. Ziaja et al. \cite{ziaja_shm_2021} &amp; 16 \\</v>
+        <f>D11&amp;" \cite{"&amp;VLOOKUP(F11,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E11 &amp; " \\"</f>
+        <v>D. Ziaja et al. \cite{4} &amp; 16 \\</v>
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
@@ -3768,8 +3974,8 @@
         <v>13</v>
       </c>
       <c r="I12" t="str">
-        <f>D12&amp;" \cite{"&amp;VLOOKUP(F12,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E12 &amp; " \\"</f>
-        <v>X. F. Sánchez-Romate et al. \cite{sanchez-romate_structural_2021} &amp; 16 \\</v>
+        <f>D12&amp;" \cite{"&amp;VLOOKUP(F12,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E12 &amp; " \\"</f>
+        <v>X. F. Sánchez-Romate et al. \cite{10} &amp; 16 \\</v>
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
@@ -3783,8 +3989,8 @@
         <v>30</v>
       </c>
       <c r="I13" t="str">
-        <f>D13&amp;" \cite{"&amp;VLOOKUP(F13,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E13 &amp; " \\"</f>
-        <v>B. Zima \cite{zima_damage_2021} &amp; 15 \\</v>
+        <f>D13&amp;" \cite{"&amp;VLOOKUP(F13,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E13 &amp; " \\"</f>
+        <v>B. Zima \cite{25} &amp; 15 \\</v>
       </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
@@ -3798,8 +4004,8 @@
         <v>5</v>
       </c>
       <c r="I14" t="str">
-        <f>D14&amp;" \cite{"&amp;VLOOKUP(F14,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E14 &amp; " \\"</f>
-        <v>M. Moradi et al. \cite{moradi_intelligent_2023} &amp; 14 \\</v>
+        <f>D14&amp;" \cite{"&amp;VLOOKUP(F14,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E14 &amp; " \\"</f>
+        <v>M. Moradi et al. \cite{3} &amp; 14 \\</v>
       </c>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
@@ -3813,8 +4019,8 @@
         <v>19</v>
       </c>
       <c r="I15" t="str">
-        <f>D15&amp;" \cite{"&amp;VLOOKUP(F15,sorted_references_linked!A:C,3,FALSE) &amp; "} &amp; " &amp; E15 &amp; " \\"</f>
-        <v>Y. Dong et al. \cite{dong_ultrasonic_2022} &amp; 10 \\</v>
+        <f>D15&amp;" \cite{"&amp;VLOOKUP(F15,sorted_references_linked!A:D,3,FALSE) &amp; "} &amp; " &amp; E15 &amp; " \\"</f>
+        <v>Y. Dong et al. \cite{16} &amp; 10 \\</v>
       </c>
     </row>
   </sheetData>

</xml_diff>